<commit_message>
Mistake in construction fix
</commit_message>
<xml_diff>
--- a/Stimuli/Copy of Constructions Corpus.xlsx
+++ b/Stimuli/Copy of Constructions Corpus.xlsx
@@ -93,9 +93,6 @@
     <t>BCA,BAC</t>
   </si>
   <si>
-    <t xml:space="preserve">BCA </t>
-  </si>
-  <si>
     <t>Infont of</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Non-Ambiguous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBA </t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:H36"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,22 +596,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>35</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
       </c>
       <c r="G8" t="s">
         <v>16</v>
@@ -825,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>2</v>
       </c>
       <c r="H18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -868,7 +868,7 @@
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
@@ -920,7 +920,7 @@
         <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
@@ -937,7 +937,7 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -963,7 +963,7 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -972,7 +972,7 @@
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F23" t="s">
         <v>5</v>
@@ -981,7 +981,7 @@
         <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -989,7 +989,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -1015,7 +1015,7 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -1024,7 +1024,7 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
@@ -1033,32 +1033,32 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
       </c>
       <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
         <v>33</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>34</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>35</v>
-      </c>
-      <c r="F27" t="s">
-        <v>36</v>
       </c>
       <c r="G27" t="s">
         <v>16</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1277,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>